<commit_message>
fix industry of level 2 bugs
</commit_message>
<xml_diff>
--- a/FactorLib/resource/level_2_industry_dict.xlsx
+++ b/FactorLib/resource/level_2_industry_dict.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="18625"/>
   <workbookPr filterPrivacy="1" codeName="ThisWorkbook" defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="90" windowWidth="19200" windowHeight="11640"/>
+    <workbookView xWindow="0" yWindow="90" windowWidth="19200" windowHeight="11640" activeTab="2"/>
   </bookViews>
   <sheets>
     <sheet name="sw_level_2" sheetId="1" r:id="rId1"/>
@@ -17,7 +17,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="504" uniqueCount="475">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="516" uniqueCount="487">
   <si>
     <t>林业Ⅱ</t>
   </si>
@@ -1124,9 +1124,6 @@
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
-    <t>801780</t>
-  </si>
-  <si>
     <t>农林牧渔</t>
   </si>
   <si>
@@ -1506,6 +1503,58 @@
   </si>
   <si>
     <t>CI005167</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>801060</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>建筑建材</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>801070</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>机械设备</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>801090</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>交运设备</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>801190</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>金融服务</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>801100</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>信息设备</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>801220</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>信息服务</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>801192</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
 </sst>
@@ -1552,7 +1601,7 @@
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="4">
+  <cellXfs count="5">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
       <alignment vertical="center"/>
     </xf>
@@ -1564,6 +1613,9 @@
     </xf>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyNumberFormat="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -1906,8 +1958,8 @@
   <sheetPr codeName="Sheet1"/>
   <dimension ref="A1:B105"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B15" sqref="B15"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B12" sqref="B12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.5" x14ac:dyDescent="0.15"/>
@@ -3544,10 +3596,10 @@
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <sheetPr codeName="Sheet3"/>
-  <dimension ref="A1:B31"/>
+  <dimension ref="A1:B37"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A5" sqref="A5"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="I13" sqref="I13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.5" x14ac:dyDescent="0.15"/>
@@ -3565,7 +3617,7 @@
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.15">
       <c r="A2" s="1" t="s">
-        <v>366</v>
+        <v>486</v>
       </c>
       <c r="B2" s="1" t="s">
         <v>363</v>
@@ -3592,215 +3644,263 @@
         <v>325</v>
       </c>
       <c r="B5" s="1" t="s">
-        <v>370</v>
+        <v>369</v>
       </c>
     </row>
     <row r="6" spans="1:2" x14ac:dyDescent="0.15">
       <c r="A6" s="1" t="s">
-        <v>397</v>
+        <v>396</v>
       </c>
       <c r="B6" s="1" t="s">
-        <v>371</v>
+        <v>370</v>
       </c>
     </row>
     <row r="7" spans="1:2" x14ac:dyDescent="0.15">
       <c r="A7" s="1" t="s">
-        <v>398</v>
+        <v>397</v>
       </c>
       <c r="B7" s="1" t="s">
-        <v>372</v>
+        <v>371</v>
       </c>
     </row>
     <row r="8" spans="1:2" x14ac:dyDescent="0.15">
       <c r="A8" s="1" t="s">
-        <v>399</v>
+        <v>398</v>
       </c>
       <c r="B8" s="1" t="s">
-        <v>373</v>
+        <v>372</v>
       </c>
     </row>
     <row r="9" spans="1:2" x14ac:dyDescent="0.15">
       <c r="A9" s="1" t="s">
-        <v>400</v>
+        <v>399</v>
       </c>
       <c r="B9" s="1" t="s">
-        <v>374</v>
+        <v>373</v>
       </c>
     </row>
     <row r="10" spans="1:2" x14ac:dyDescent="0.15">
       <c r="A10" s="1" t="s">
-        <v>401</v>
+        <v>400</v>
       </c>
       <c r="B10" s="1" t="s">
-        <v>375</v>
+        <v>374</v>
       </c>
     </row>
     <row r="11" spans="1:2" x14ac:dyDescent="0.15">
       <c r="A11" s="1" t="s">
-        <v>402</v>
+        <v>401</v>
       </c>
       <c r="B11" s="1" t="s">
-        <v>376</v>
+        <v>375</v>
       </c>
     </row>
     <row r="12" spans="1:2" x14ac:dyDescent="0.15">
       <c r="A12" s="1" t="s">
-        <v>403</v>
+        <v>402</v>
       </c>
       <c r="B12" s="1" t="s">
-        <v>377</v>
+        <v>376</v>
       </c>
     </row>
     <row r="13" spans="1:2" x14ac:dyDescent="0.15">
       <c r="A13" s="1" t="s">
-        <v>404</v>
+        <v>403</v>
       </c>
       <c r="B13" s="1" t="s">
-        <v>378</v>
+        <v>377</v>
       </c>
     </row>
     <row r="14" spans="1:2" x14ac:dyDescent="0.15">
       <c r="A14" s="1" t="s">
-        <v>405</v>
+        <v>404</v>
       </c>
       <c r="B14" s="1" t="s">
-        <v>379</v>
+        <v>378</v>
       </c>
     </row>
     <row r="15" spans="1:2" x14ac:dyDescent="0.15">
       <c r="A15" s="1" t="s">
-        <v>406</v>
+        <v>405</v>
       </c>
       <c r="B15" s="1" t="s">
-        <v>380</v>
+        <v>379</v>
       </c>
     </row>
     <row r="16" spans="1:2" x14ac:dyDescent="0.15">
       <c r="A16" s="1" t="s">
-        <v>407</v>
+        <v>406</v>
       </c>
       <c r="B16" s="1" t="s">
-        <v>381</v>
+        <v>380</v>
       </c>
     </row>
     <row r="17" spans="1:2" x14ac:dyDescent="0.15">
       <c r="A17" s="1" t="s">
-        <v>408</v>
+        <v>407</v>
       </c>
       <c r="B17" s="1" t="s">
-        <v>382</v>
+        <v>381</v>
       </c>
     </row>
     <row r="18" spans="1:2" x14ac:dyDescent="0.15">
       <c r="A18" s="1" t="s">
-        <v>409</v>
+        <v>408</v>
       </c>
       <c r="B18" s="1" t="s">
-        <v>383</v>
+        <v>382</v>
       </c>
     </row>
     <row r="19" spans="1:2" x14ac:dyDescent="0.15">
       <c r="A19" s="1" t="s">
-        <v>410</v>
+        <v>409</v>
       </c>
       <c r="B19" s="1" t="s">
-        <v>384</v>
+        <v>383</v>
       </c>
     </row>
     <row r="20" spans="1:2" x14ac:dyDescent="0.15">
       <c r="A20" s="1" t="s">
-        <v>411</v>
+        <v>410</v>
       </c>
       <c r="B20" s="1" t="s">
-        <v>385</v>
+        <v>384</v>
       </c>
     </row>
     <row r="21" spans="1:2" x14ac:dyDescent="0.15">
       <c r="A21" s="1" t="s">
-        <v>412</v>
+        <v>411</v>
       </c>
       <c r="B21" s="1" t="s">
-        <v>386</v>
+        <v>385</v>
       </c>
     </row>
     <row r="22" spans="1:2" x14ac:dyDescent="0.15">
       <c r="A22" s="1" t="s">
-        <v>413</v>
+        <v>412</v>
       </c>
       <c r="B22" s="1" t="s">
-        <v>387</v>
+        <v>386</v>
       </c>
     </row>
     <row r="23" spans="1:2" x14ac:dyDescent="0.15">
       <c r="A23" s="1" t="s">
-        <v>414</v>
+        <v>413</v>
       </c>
       <c r="B23" s="1" t="s">
-        <v>388</v>
+        <v>387</v>
       </c>
     </row>
     <row r="24" spans="1:2" x14ac:dyDescent="0.15">
       <c r="A24" s="1" t="s">
-        <v>415</v>
+        <v>414</v>
       </c>
       <c r="B24" s="1" t="s">
-        <v>389</v>
+        <v>388</v>
       </c>
     </row>
     <row r="25" spans="1:2" x14ac:dyDescent="0.15">
       <c r="A25" s="1" t="s">
-        <v>416</v>
+        <v>415</v>
       </c>
       <c r="B25" s="1" t="s">
-        <v>390</v>
+        <v>389</v>
       </c>
     </row>
     <row r="26" spans="1:2" x14ac:dyDescent="0.15">
       <c r="A26" s="1" t="s">
-        <v>417</v>
+        <v>416</v>
       </c>
       <c r="B26" s="1" t="s">
-        <v>391</v>
+        <v>390</v>
       </c>
     </row>
     <row r="27" spans="1:2" x14ac:dyDescent="0.15">
       <c r="A27" s="1" t="s">
-        <v>418</v>
+        <v>417</v>
       </c>
       <c r="B27" s="1" t="s">
-        <v>392</v>
+        <v>391</v>
       </c>
     </row>
     <row r="28" spans="1:2" x14ac:dyDescent="0.15">
       <c r="A28" s="1" t="s">
-        <v>419</v>
+        <v>418</v>
       </c>
       <c r="B28" s="1" t="s">
-        <v>393</v>
+        <v>392</v>
       </c>
     </row>
     <row r="29" spans="1:2" x14ac:dyDescent="0.15">
       <c r="A29" s="1" t="s">
-        <v>420</v>
+        <v>419</v>
       </c>
       <c r="B29" s="1" t="s">
-        <v>394</v>
+        <v>393</v>
       </c>
     </row>
     <row r="30" spans="1:2" x14ac:dyDescent="0.15">
       <c r="A30" s="1" t="s">
-        <v>421</v>
+        <v>420</v>
       </c>
       <c r="B30" s="1" t="s">
-        <v>395</v>
+        <v>394</v>
       </c>
     </row>
     <row r="31" spans="1:2" x14ac:dyDescent="0.15">
       <c r="A31" s="1" t="s">
-        <v>422</v>
+        <v>421</v>
       </c>
       <c r="B31" s="1" t="s">
-        <v>396</v>
+        <v>395</v>
+      </c>
+    </row>
+    <row r="32" spans="1:2" x14ac:dyDescent="0.15">
+      <c r="A32" s="4" t="s">
+        <v>474</v>
+      </c>
+      <c r="B32" s="1" t="s">
+        <v>475</v>
+      </c>
+    </row>
+    <row r="33" spans="1:2" x14ac:dyDescent="0.15">
+      <c r="A33" s="4" t="s">
+        <v>476</v>
+      </c>
+      <c r="B33" s="1" t="s">
+        <v>477</v>
+      </c>
+    </row>
+    <row r="34" spans="1:2" x14ac:dyDescent="0.15">
+      <c r="A34" s="4" t="s">
+        <v>478</v>
+      </c>
+      <c r="B34" s="1" t="s">
+        <v>479</v>
+      </c>
+    </row>
+    <row r="35" spans="1:2" x14ac:dyDescent="0.15">
+      <c r="A35" s="4" t="s">
+        <v>480</v>
+      </c>
+      <c r="B35" s="1" t="s">
+        <v>481</v>
+      </c>
+    </row>
+    <row r="36" spans="1:2" x14ac:dyDescent="0.15">
+      <c r="A36" s="4" t="s">
+        <v>482</v>
+      </c>
+      <c r="B36" s="1" t="s">
+        <v>483</v>
+      </c>
+    </row>
+    <row r="37" spans="1:2" x14ac:dyDescent="0.15">
+      <c r="A37" s="4" t="s">
+        <v>484</v>
+      </c>
+      <c r="B37" s="1" t="s">
+        <v>485</v>
       </c>
     </row>
   </sheetData>
@@ -3812,6 +3912,7 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <sheetPr codeName="Sheet4"/>
   <dimension ref="A1:B32"/>
   <sheetViews>
     <sheetView workbookViewId="0">
@@ -3834,23 +3935,23 @@
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.15">
       <c r="A2" s="3" t="s">
-        <v>472</v>
+        <v>471</v>
       </c>
       <c r="B2" s="3" t="s">
-        <v>423</v>
+        <v>422</v>
       </c>
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.15">
       <c r="A3" s="3" t="s">
-        <v>473</v>
+        <v>472</v>
       </c>
       <c r="B3" s="3" t="s">
-        <v>424</v>
+        <v>423</v>
       </c>
     </row>
     <row r="4" spans="1:2" x14ac:dyDescent="0.15">
       <c r="A4" s="3" t="s">
-        <v>474</v>
+        <v>473</v>
       </c>
       <c r="B4" s="3" t="s">
         <v>154</v>
@@ -3858,167 +3959,167 @@
     </row>
     <row r="5" spans="1:2" x14ac:dyDescent="0.15">
       <c r="A5" s="2" t="s">
+        <v>449</v>
+      </c>
+      <c r="B5" s="2" t="s">
         <v>450</v>
-      </c>
-      <c r="B5" s="2" t="s">
-        <v>451</v>
       </c>
     </row>
     <row r="6" spans="1:2" x14ac:dyDescent="0.15">
       <c r="A6" s="3" t="s">
-        <v>425</v>
+        <v>424</v>
       </c>
       <c r="B6" s="3" t="s">
-        <v>452</v>
+        <v>451</v>
       </c>
     </row>
     <row r="7" spans="1:2" x14ac:dyDescent="0.15">
       <c r="A7" s="3" t="s">
-        <v>426</v>
+        <v>425</v>
       </c>
       <c r="B7" s="3" t="s">
-        <v>453</v>
+        <v>452</v>
       </c>
     </row>
     <row r="8" spans="1:2" x14ac:dyDescent="0.15">
       <c r="A8" s="3" t="s">
+        <v>426</v>
+      </c>
+      <c r="B8" s="3" t="s">
         <v>427</v>
-      </c>
-      <c r="B8" s="3" t="s">
-        <v>428</v>
       </c>
     </row>
     <row r="9" spans="1:2" x14ac:dyDescent="0.15">
       <c r="A9" s="2" t="s">
-        <v>454</v>
+        <v>453</v>
       </c>
       <c r="B9" s="2" t="s">
-        <v>374</v>
+        <v>373</v>
       </c>
     </row>
     <row r="10" spans="1:2" x14ac:dyDescent="0.15">
       <c r="A10" s="3" t="s">
-        <v>429</v>
+        <v>428</v>
       </c>
       <c r="B10" s="3" t="s">
-        <v>455</v>
+        <v>454</v>
       </c>
     </row>
     <row r="11" spans="1:2" x14ac:dyDescent="0.15">
       <c r="A11" s="3" t="s">
-        <v>430</v>
+        <v>429</v>
       </c>
       <c r="B11" s="3" t="s">
-        <v>456</v>
+        <v>455</v>
       </c>
     </row>
     <row r="12" spans="1:2" x14ac:dyDescent="0.15">
       <c r="A12" s="3" t="s">
+        <v>430</v>
+      </c>
+      <c r="B12" s="3" t="s">
         <v>431</v>
-      </c>
-      <c r="B12" s="3" t="s">
-        <v>432</v>
       </c>
     </row>
     <row r="13" spans="1:2" x14ac:dyDescent="0.15">
       <c r="A13" s="2" t="s">
-        <v>457</v>
+        <v>456</v>
       </c>
       <c r="B13" s="2" t="s">
-        <v>380</v>
+        <v>379</v>
       </c>
     </row>
     <row r="14" spans="1:2" x14ac:dyDescent="0.15">
       <c r="A14" s="3" t="s">
-        <v>433</v>
+        <v>432</v>
       </c>
       <c r="B14" s="3" t="s">
-        <v>458</v>
+        <v>457</v>
       </c>
     </row>
     <row r="15" spans="1:2" x14ac:dyDescent="0.15">
       <c r="A15" s="3" t="s">
-        <v>434</v>
+        <v>433</v>
       </c>
       <c r="B15" s="3" t="s">
-        <v>459</v>
+        <v>458</v>
       </c>
     </row>
     <row r="16" spans="1:2" x14ac:dyDescent="0.15">
       <c r="A16" s="3" t="s">
-        <v>435</v>
+        <v>434</v>
       </c>
       <c r="B16" s="3" t="s">
-        <v>369</v>
+        <v>368</v>
       </c>
     </row>
     <row r="17" spans="1:2" x14ac:dyDescent="0.15">
       <c r="A17" s="2" t="s">
-        <v>460</v>
+        <v>459</v>
       </c>
       <c r="B17" s="2" t="s">
-        <v>395</v>
+        <v>394</v>
       </c>
     </row>
     <row r="18" spans="1:2" x14ac:dyDescent="0.15">
       <c r="A18" s="3" t="s">
-        <v>436</v>
+        <v>435</v>
       </c>
       <c r="B18" s="3" t="s">
-        <v>461</v>
+        <v>460</v>
       </c>
     </row>
     <row r="19" spans="1:2" x14ac:dyDescent="0.15">
       <c r="A19" s="3" t="s">
-        <v>437</v>
+        <v>436</v>
       </c>
       <c r="B19" s="3" t="s">
-        <v>462</v>
+        <v>461</v>
       </c>
     </row>
     <row r="20" spans="1:2" x14ac:dyDescent="0.15">
       <c r="A20" s="3" t="s">
+        <v>437</v>
+      </c>
+      <c r="B20" s="3" t="s">
         <v>438</v>
-      </c>
-      <c r="B20" s="3" t="s">
-        <v>439</v>
       </c>
     </row>
     <row r="21" spans="1:2" x14ac:dyDescent="0.15">
       <c r="A21" s="2" t="s">
-        <v>463</v>
+        <v>462</v>
       </c>
       <c r="B21" s="2" t="s">
-        <v>379</v>
+        <v>378</v>
       </c>
     </row>
     <row r="22" spans="1:2" x14ac:dyDescent="0.15">
       <c r="A22" s="3" t="s">
-        <v>440</v>
+        <v>439</v>
       </c>
       <c r="B22" s="3" t="s">
-        <v>464</v>
+        <v>463</v>
       </c>
     </row>
     <row r="23" spans="1:2" x14ac:dyDescent="0.15">
       <c r="A23" s="3" t="s">
-        <v>441</v>
+        <v>440</v>
       </c>
       <c r="B23" s="3" t="s">
-        <v>465</v>
+        <v>464</v>
       </c>
     </row>
     <row r="24" spans="1:2" x14ac:dyDescent="0.15">
       <c r="A24" s="3" t="s">
-        <v>442</v>
+        <v>441</v>
       </c>
       <c r="B24" s="3" t="s">
-        <v>367</v>
+        <v>366</v>
       </c>
     </row>
     <row r="25" spans="1:2" x14ac:dyDescent="0.15">
       <c r="A25" s="2" t="s">
-        <v>466</v>
+        <v>465</v>
       </c>
       <c r="B25" s="2" t="s">
         <v>363</v>
@@ -4026,58 +4127,58 @@
     </row>
     <row r="26" spans="1:2" x14ac:dyDescent="0.15">
       <c r="A26" s="3" t="s">
-        <v>443</v>
+        <v>442</v>
       </c>
       <c r="B26" s="3" t="s">
-        <v>467</v>
+        <v>466</v>
       </c>
     </row>
     <row r="27" spans="1:2" x14ac:dyDescent="0.15">
       <c r="A27" s="3" t="s">
-        <v>444</v>
+        <v>443</v>
       </c>
       <c r="B27" s="3" t="s">
-        <v>468</v>
+        <v>467</v>
       </c>
     </row>
     <row r="28" spans="1:2" x14ac:dyDescent="0.15">
       <c r="A28" s="3" t="s">
+        <v>444</v>
+      </c>
+      <c r="B28" s="3" t="s">
         <v>445</v>
-      </c>
-      <c r="B28" s="3" t="s">
-        <v>446</v>
       </c>
     </row>
     <row r="29" spans="1:2" x14ac:dyDescent="0.15">
       <c r="A29" s="2" t="s">
-        <v>469</v>
+        <v>468</v>
       </c>
       <c r="B29" s="2" t="s">
-        <v>394</v>
+        <v>393</v>
       </c>
     </row>
     <row r="30" spans="1:2" x14ac:dyDescent="0.15">
       <c r="A30" s="3" t="s">
-        <v>447</v>
+        <v>446</v>
       </c>
       <c r="B30" s="3" t="s">
-        <v>470</v>
+        <v>469</v>
       </c>
     </row>
     <row r="31" spans="1:2" x14ac:dyDescent="0.15">
       <c r="A31" s="3" t="s">
-        <v>448</v>
+        <v>447</v>
       </c>
       <c r="B31" s="3" t="s">
-        <v>471</v>
+        <v>470</v>
       </c>
     </row>
     <row r="32" spans="1:2" x14ac:dyDescent="0.15">
       <c r="A32" s="3" t="s">
-        <v>449</v>
+        <v>448</v>
       </c>
       <c r="B32" s="3" t="s">
-        <v>368</v>
+        <v>367</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
commit before modify hdf5 file store mode
</commit_message>
<xml_diff>
--- a/FactorLib/resource/level_2_industry_dict.xlsx
+++ b/FactorLib/resource/level_2_industry_dict.xlsx
@@ -1,11 +1,11 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="21425"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="22325"/>
   <workbookPr filterPrivacy="1" codeName="ThisWorkbook" defaultThemeVersion="124226"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4B48706E-CD81-42B6-A2A2-332D4D56D750}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{43CBC1E2-B9F4-40C9-BCC7-1C86E3C1187F}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-30828" yWindow="-108" windowWidth="30936" windowHeight="16896" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="sw_level_2" sheetId="1" r:id="rId1"/>
@@ -1707,9 +1707,6 @@
     <t>机械</t>
   </si>
   <si>
-    <t>电力设备</t>
-  </si>
-  <si>
     <t>CI005013</t>
   </si>
   <si>
@@ -1719,9 +1716,6 @@
     <t>CI005015</t>
   </si>
   <si>
-    <t>餐饮旅游</t>
-  </si>
-  <si>
     <t>CI005017</t>
   </si>
   <si>
@@ -1942,6 +1936,14 @@
   </si>
   <si>
     <t>其他采掘Ⅱ</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>电力设备及新能源</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>消费者服务</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
 </sst>
@@ -2372,7 +2374,7 @@
   <sheetPr codeName="Sheet1"/>
   <dimension ref="A1:B105"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A49" workbookViewId="0">
+    <sheetView topLeftCell="A49" workbookViewId="0">
       <selection activeCell="B11" sqref="B11"/>
     </sheetView>
   </sheetViews>
@@ -2467,7 +2469,7 @@
         <v>265</v>
       </c>
       <c r="B11" s="1" t="s">
-        <v>613</v>
+        <v>611</v>
       </c>
     </row>
     <row r="12" spans="1:2" x14ac:dyDescent="0.15">
@@ -3529,11 +3531,15 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{755319A0-1E58-473C-80F5-D820273C9363}">
   <dimension ref="A1:B30"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A2" sqref="A2"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="F23" sqref="F23"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.5" x14ac:dyDescent="0.15"/>
+  <cols>
+    <col min="1" max="1" width="10.75" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="15.125" bestFit="1" customWidth="1"/>
+  </cols>
   <sheetData>
     <row r="1" spans="1:2" x14ac:dyDescent="0.15">
       <c r="A1" s="6" t="s">
@@ -3628,7 +3634,7 @@
         <v>432</v>
       </c>
       <c r="B12" s="6" t="s">
-        <v>535</v>
+        <v>612</v>
       </c>
     </row>
     <row r="13" spans="1:2" x14ac:dyDescent="0.15">
@@ -3641,7 +3647,7 @@
     </row>
     <row r="14" spans="1:2" x14ac:dyDescent="0.15">
       <c r="A14" s="5" t="s">
-        <v>536</v>
+        <v>535</v>
       </c>
       <c r="B14" s="6" t="s">
         <v>512</v>
@@ -3652,15 +3658,15 @@
         <v>434</v>
       </c>
       <c r="B15" s="6" t="s">
-        <v>537</v>
+        <v>536</v>
       </c>
     </row>
     <row r="16" spans="1:2" x14ac:dyDescent="0.15">
       <c r="A16" s="5" t="s">
-        <v>538</v>
+        <v>537</v>
       </c>
       <c r="B16" s="6" t="s">
-        <v>539</v>
+        <v>613</v>
       </c>
     </row>
     <row r="17" spans="1:2" x14ac:dyDescent="0.15">
@@ -3673,7 +3679,7 @@
     </row>
     <row r="18" spans="1:2" x14ac:dyDescent="0.15">
       <c r="A18" s="5" t="s">
-        <v>540</v>
+        <v>538</v>
       </c>
       <c r="B18" s="6" t="s">
         <v>494</v>
@@ -3684,12 +3690,12 @@
         <v>438</v>
       </c>
       <c r="B19" s="6" t="s">
-        <v>541</v>
+        <v>539</v>
       </c>
     </row>
     <row r="20" spans="1:2" x14ac:dyDescent="0.15">
       <c r="A20" s="5" t="s">
-        <v>542</v>
+        <v>540</v>
       </c>
       <c r="B20" s="6" t="s">
         <v>493</v>
@@ -3705,7 +3711,7 @@
     </row>
     <row r="22" spans="1:2" x14ac:dyDescent="0.15">
       <c r="A22" s="5" t="s">
-        <v>543</v>
+        <v>541</v>
       </c>
       <c r="B22" s="6" t="s">
         <v>509</v>
@@ -3713,10 +3719,10 @@
     </row>
     <row r="23" spans="1:2" x14ac:dyDescent="0.15">
       <c r="A23" s="5" t="s">
-        <v>544</v>
+        <v>542</v>
       </c>
       <c r="B23" s="6" t="s">
-        <v>545</v>
+        <v>543</v>
       </c>
     </row>
     <row r="24" spans="1:2" x14ac:dyDescent="0.15">
@@ -3740,12 +3746,12 @@
         <v>443</v>
       </c>
       <c r="B26" s="6" t="s">
-        <v>444</v>
+        <v>374</v>
       </c>
     </row>
     <row r="27" spans="1:2" x14ac:dyDescent="0.15">
       <c r="A27" s="5" t="s">
-        <v>546</v>
+        <v>544</v>
       </c>
       <c r="B27" s="6" t="s">
         <v>507</v>
@@ -4579,79 +4585,79 @@
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.15">
       <c r="A2" s="5" t="s">
-        <v>547</v>
+        <v>545</v>
       </c>
       <c r="B2" s="6" t="s">
-        <v>548</v>
+        <v>546</v>
       </c>
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.15">
       <c r="A3" s="5" t="s">
-        <v>549</v>
+        <v>547</v>
       </c>
       <c r="B3" s="6" t="s">
-        <v>550</v>
+        <v>548</v>
       </c>
     </row>
     <row r="4" spans="1:2" x14ac:dyDescent="0.15">
       <c r="A4" s="5" t="s">
-        <v>551</v>
+        <v>549</v>
       </c>
       <c r="B4" s="6" t="s">
-        <v>552</v>
+        <v>550</v>
       </c>
     </row>
     <row r="5" spans="1:2" x14ac:dyDescent="0.15">
       <c r="A5" s="5" t="s">
-        <v>553</v>
+        <v>551</v>
       </c>
       <c r="B5" s="6" t="s">
-        <v>554</v>
+        <v>552</v>
       </c>
     </row>
     <row r="6" spans="1:2" x14ac:dyDescent="0.15">
       <c r="A6" s="5" t="s">
-        <v>555</v>
+        <v>553</v>
       </c>
       <c r="B6" s="6" t="s">
-        <v>556</v>
+        <v>554</v>
       </c>
     </row>
     <row r="7" spans="1:2" x14ac:dyDescent="0.15">
       <c r="A7" s="5" t="s">
-        <v>557</v>
+        <v>555</v>
       </c>
       <c r="B7" s="6" t="s">
-        <v>558</v>
+        <v>556</v>
       </c>
     </row>
     <row r="8" spans="1:2" x14ac:dyDescent="0.15">
       <c r="A8" s="5" t="s">
-        <v>559</v>
+        <v>557</v>
       </c>
       <c r="B8" s="6" t="s">
-        <v>560</v>
+        <v>558</v>
       </c>
     </row>
     <row r="9" spans="1:2" x14ac:dyDescent="0.15">
       <c r="A9" s="5" t="s">
-        <v>561</v>
+        <v>559</v>
       </c>
       <c r="B9" s="6" t="s">
-        <v>562</v>
+        <v>560</v>
       </c>
     </row>
     <row r="10" spans="1:2" x14ac:dyDescent="0.15">
       <c r="A10" s="5" t="s">
-        <v>563</v>
+        <v>561</v>
       </c>
       <c r="B10" s="6" t="s">
-        <v>564</v>
+        <v>562</v>
       </c>
     </row>
     <row r="11" spans="1:2" x14ac:dyDescent="0.15">
       <c r="A11" s="5" t="s">
-        <v>565</v>
+        <v>563</v>
       </c>
       <c r="B11" s="6" t="s">
         <v>497</v>
@@ -4659,7 +4665,7 @@
     </row>
     <row r="12" spans="1:2" x14ac:dyDescent="0.15">
       <c r="A12" s="5" t="s">
-        <v>566</v>
+        <v>564</v>
       </c>
       <c r="B12" s="6" t="s">
         <v>499</v>
@@ -4694,127 +4700,127 @@
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.15">
       <c r="A2" s="1" t="s">
-        <v>567</v>
+        <v>565</v>
       </c>
       <c r="B2" t="s">
-        <v>591</v>
+        <v>589</v>
       </c>
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.15">
       <c r="A3" s="1" t="s">
-        <v>568</v>
+        <v>566</v>
       </c>
       <c r="B3" t="s">
-        <v>592</v>
+        <v>590</v>
       </c>
     </row>
     <row r="4" spans="1:2" x14ac:dyDescent="0.15">
       <c r="A4" s="1" t="s">
-        <v>569</v>
+        <v>567</v>
       </c>
       <c r="B4" t="s">
-        <v>593</v>
+        <v>591</v>
       </c>
     </row>
     <row r="5" spans="1:2" x14ac:dyDescent="0.15">
       <c r="A5" s="1" t="s">
-        <v>570</v>
+        <v>568</v>
       </c>
       <c r="B5" t="s">
-        <v>594</v>
+        <v>592</v>
       </c>
     </row>
     <row r="6" spans="1:2" x14ac:dyDescent="0.15">
       <c r="A6" s="1" t="s">
-        <v>571</v>
+        <v>569</v>
       </c>
       <c r="B6" t="s">
-        <v>595</v>
+        <v>593</v>
       </c>
     </row>
     <row r="7" spans="1:2" x14ac:dyDescent="0.15">
       <c r="A7" s="1" t="s">
-        <v>572</v>
+        <v>570</v>
       </c>
       <c r="B7" t="s">
-        <v>596</v>
+        <v>594</v>
       </c>
     </row>
     <row r="8" spans="1:2" x14ac:dyDescent="0.15">
       <c r="A8" s="1" t="s">
-        <v>573</v>
+        <v>571</v>
       </c>
       <c r="B8" t="s">
-        <v>597</v>
+        <v>595</v>
       </c>
     </row>
     <row r="9" spans="1:2" x14ac:dyDescent="0.15">
       <c r="A9" s="1" t="s">
-        <v>574</v>
+        <v>572</v>
       </c>
       <c r="B9" t="s">
-        <v>598</v>
+        <v>596</v>
       </c>
     </row>
     <row r="10" spans="1:2" x14ac:dyDescent="0.15">
       <c r="A10" s="1" t="s">
-        <v>575</v>
+        <v>573</v>
       </c>
       <c r="B10" t="s">
-        <v>599</v>
+        <v>597</v>
       </c>
     </row>
     <row r="11" spans="1:2" x14ac:dyDescent="0.15">
       <c r="A11" s="1" t="s">
-        <v>576</v>
+        <v>574</v>
       </c>
       <c r="B11" t="s">
-        <v>600</v>
+        <v>598</v>
       </c>
     </row>
     <row r="12" spans="1:2" x14ac:dyDescent="0.15">
       <c r="A12" s="1" t="s">
-        <v>577</v>
+        <v>575</v>
       </c>
       <c r="B12" t="s">
-        <v>601</v>
+        <v>599</v>
       </c>
     </row>
     <row r="13" spans="1:2" x14ac:dyDescent="0.15">
       <c r="A13" s="1" t="s">
-        <v>578</v>
+        <v>576</v>
       </c>
       <c r="B13" t="s">
-        <v>602</v>
+        <v>600</v>
       </c>
     </row>
     <row r="14" spans="1:2" x14ac:dyDescent="0.15">
       <c r="A14" s="1" t="s">
-        <v>579</v>
+        <v>577</v>
       </c>
       <c r="B14" t="s">
-        <v>603</v>
+        <v>601</v>
       </c>
     </row>
     <row r="15" spans="1:2" x14ac:dyDescent="0.15">
       <c r="A15" s="1" t="s">
-        <v>580</v>
+        <v>578</v>
       </c>
       <c r="B15" t="s">
-        <v>604</v>
+        <v>602</v>
       </c>
     </row>
     <row r="16" spans="1:2" x14ac:dyDescent="0.15">
       <c r="A16" s="1" t="s">
-        <v>581</v>
+        <v>579</v>
       </c>
       <c r="B16" t="s">
-        <v>605</v>
+        <v>603</v>
       </c>
     </row>
     <row r="17" spans="1:2" x14ac:dyDescent="0.15">
       <c r="A17" s="1" t="s">
-        <v>582</v>
+        <v>580</v>
       </c>
       <c r="B17" t="s">
         <v>509</v>
@@ -4822,15 +4828,15 @@
     </row>
     <row r="18" spans="1:2" x14ac:dyDescent="0.15">
       <c r="A18" s="1" t="s">
-        <v>583</v>
+        <v>581</v>
       </c>
       <c r="B18" t="s">
-        <v>606</v>
+        <v>604</v>
       </c>
     </row>
     <row r="19" spans="1:2" x14ac:dyDescent="0.15">
       <c r="A19" s="1" t="s">
-        <v>584</v>
+        <v>582</v>
       </c>
       <c r="B19" t="s">
         <v>70</v>
@@ -4838,50 +4844,50 @@
     </row>
     <row r="20" spans="1:2" x14ac:dyDescent="0.15">
       <c r="A20" s="1" t="s">
-        <v>585</v>
+        <v>583</v>
       </c>
       <c r="B20" t="s">
-        <v>607</v>
+        <v>605</v>
       </c>
     </row>
     <row r="21" spans="1:2" x14ac:dyDescent="0.15">
       <c r="A21" s="1" t="s">
-        <v>586</v>
+        <v>584</v>
       </c>
       <c r="B21" t="s">
-        <v>608</v>
+        <v>606</v>
       </c>
     </row>
     <row r="22" spans="1:2" x14ac:dyDescent="0.15">
       <c r="A22" s="1" t="s">
-        <v>587</v>
+        <v>585</v>
       </c>
       <c r="B22" t="s">
-        <v>609</v>
+        <v>607</v>
       </c>
     </row>
     <row r="23" spans="1:2" x14ac:dyDescent="0.15">
       <c r="A23" s="1" t="s">
-        <v>588</v>
+        <v>586</v>
       </c>
       <c r="B23" t="s">
-        <v>610</v>
+        <v>608</v>
       </c>
     </row>
     <row r="24" spans="1:2" x14ac:dyDescent="0.15">
       <c r="A24" s="1" t="s">
-        <v>589</v>
+        <v>587</v>
       </c>
       <c r="B24" t="s">
-        <v>611</v>
+        <v>609</v>
       </c>
     </row>
     <row r="25" spans="1:2" x14ac:dyDescent="0.15">
       <c r="A25" s="1" t="s">
-        <v>590</v>
+        <v>588</v>
       </c>
       <c r="B25" t="s">
-        <v>612</v>
+        <v>610</v>
       </c>
     </row>
   </sheetData>

</xml_diff>